<commit_message>
Aligned img names with doc, added test data, img and sensor info.
</commit_message>
<xml_diff>
--- a/MAP Sensor Data.xlsx
+++ b/MAP Sensor Data.xlsx
@@ -8,24 +8,19 @@
   </bookViews>
   <sheets>
     <sheet name="ATM Data" sheetId="6" r:id="rId1"/>
-    <sheet name="DENSO - Honda PS-33" sheetId="1" r:id="rId2"/>
-    <sheet name="HITACHI - PS60-01" sheetId="2" r:id="rId3"/>
-    <sheet name="DENSO 12R-3" sheetId="3" r:id="rId4"/>
-    <sheet name="OKI ELECTRIC" sheetId="4" r:id="rId5"/>
-    <sheet name="DENSO - 10M02" sheetId="5" r:id="rId6"/>
+    <sheet name="DENSO - Honda PS-30" sheetId="7" r:id="rId2"/>
+    <sheet name="DENSO - Honda PS-33" sheetId="1" r:id="rId3"/>
+    <sheet name="HITACHI - Subaru PS60-01" sheetId="2" r:id="rId4"/>
+    <sheet name="DENSO - Subaru 12R13" sheetId="3" r:id="rId5"/>
+    <sheet name="OKI - Honda MNS-151" sheetId="4" r:id="rId6"/>
+    <sheet name="DENSO - Toyota 10M02" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <webPublishObjects count="4">
-    <webPublishObject id="1940" divId="MAP Sensor Data_1940" destinationFile="C:\Users\el_presto\Desktop\WorkSpace\FreeEMS\MAP_SensorData.mht" autoRepublish="1"/>
-    <webPublishObject id="3248" divId="MAP Sensor Data_3248" destinationFile="C:\Users\el_presto\Desktop\WorkSpace\FreeEMS\OEM_MAP_SensorData.mht" autoRepublish="1"/>
-    <webPublishObject id="6926" divId="MAP Sensor Data_6926" destinationFile="C:\Users\el_presto\Desktop\WorkSpace\FreeEMS\OEMMAPweb.mht" autoRepublish="1"/>
-    <webPublishObject id="15908" divId="MAP Sensor Data_15908" destinationFile="C:\Users\el_presto\Desktop\WorkSpace\FreeEMS\OEM_MapSensors\MapSensorData.mht" title="OEM Map Sensor Data" autoRepublish="1"/>
-  </webPublishObjects>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="18">
   <si>
     <t>hPa</t>
   </si>
@@ -49,17 +44,6 @@
   </si>
   <si>
     <t>Measured</t>
-  </si>
-  <si>
-    <t>**Testing Notes**</t>
-  </si>
-  <si>
-    <t>**Testing Notes**
- - Donner vehicle = Honda NA engine (Manifold/throttle body mounted)</t>
-  </si>
-  <si>
-    <t>**Testing Notes**
- - Donner vehicle = Subaru legacy turbo engine (located on right strut tower)</t>
   </si>
   <si>
     <t>**Testing Notes**
@@ -138,6 +122,260 @@
       <t xml:space="preserve"> field above, this information can be obtained from a barometer or a local weather station webpage. </t>
     </r>
   </si>
+  <si>
+    <t>Sensor_img\DENSO_Honda_PS-33.JPG</t>
+  </si>
+  <si>
+    <t>Sensor_img\DENSO_Honda_PS-30.JPG</t>
+  </si>
+  <si>
+    <t>**Testing Notes**
+ - Donner vehicle = Honda NA engine (Manifold/throttle body mounted)
+ - Part #</t>
+  </si>
+  <si>
+    <t>**Testing Notes**
+ - Donner vehicle = Subaru legacy turbo engine (located on right strut tower)
+ - Part # PS60-01 7704
+ - Voltage rating: 5V
+ - Colour Coding :
+                     - Red (R ) = +5V
+                     - Black (B) = GND
+                     - Green (G) = Vout
+ - Measured Resistance Readings : 
+                     - R ---&gt; G = 15.3kΩ
+                     - R ---&gt; B = 3.44kΩ
+                     - G ---&gt; B = 15.9kΩ
+- MAP Test date : 24-12-2011 @ 2230hrs : 1022 hPa</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">**Testing Notes**
+ - Donner vehicle = Subaru legacy turbo engine (located on right strut tower)
+ - Part # PS60-01 7704
+ - Voltage rating: 5V
+ - Colour Coding :
+                     - Black </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>with</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Yellow Strip (BY) =GND
+                     - Yellow </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>with</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Black Strip (YB) = Vout
+                     - Red (R) = +5V
+ - Measured Resistance Readings : 
+                     - BY ---&gt; YB = 7.46kΩ
+                     - BY ---&gt; R = 3.64kΩ
+                     - YB ---&gt; R = 7.82kΩ
+- MAP Test date : 24-12-2011 @ 2400hrs : 1022 hPa</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">**Testing Notes**
+ - Donner vehicle = Honda NA engine (Mounted against front left strut)
+ - Part # MNS-151 3Z104
+ - Voltage rating: 5V
+ - Wire colour coding :
+                   - Yellow </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>with</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> White Strip (YW) = V+
+                   - Green </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>with</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> White Strip (GW) = GND
+                   - White </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>with</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Yellow Strip (WY) = Vout
+- Measured Resistance Readings :
+                   - YW ---&gt; GW = 6.04kΩ
+                   - YW ---&gt; WY = 11.74kΩ
+                   - GW ---&gt; WY = 10.07kΩ
+- MAP Test date : 24-12-2011 @ 2130hrs : 1022 hPa</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">**Testing Notes**
+ - Donner vehicle = Honda NA engine (Manifold/throttle body mounted)
+ - Part # 079800-4250
+ - Voltage rating: 5V
+ - Wire colour coding :
+                   - Red </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>with</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Green Strip (RG) = V+
+                   - Yellow </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>with</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Red Strip (YR) = Vout
+                   - Greenn </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>with</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> White Strip (GW) = GND
+- Measured Resistance Readings :
+                   - RG ---&gt; YR = 2.17k</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Ω
+                   - RG ---&gt; GW = 5.94kΩ
+                   - YR ---&gt; GW = 4.00kΩ
+- MAP Test date : 24-12-2011 @ 2300hrs : 1022 hPa</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -147,7 +385,7 @@
     <numFmt numFmtId="164" formatCode="0.00_ ;[Red]\-0.00\ "/>
     <numFmt numFmtId="165" formatCode="0_ ;[Red]\-0\ "/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +416,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -350,10 +602,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -389,6 +642,9 @@
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -422,8 +678,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -461,7 +725,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'DENSO - Honda PS-33'!$D$2</c:f>
+              <c:f>'DENSO - Honda PS-30'!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -476,7 +740,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'DENSO - Honda PS-33'!$C$3:$C$20</c:f>
+              <c:f>'DENSO - Honda PS-30'!$C$3:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>0_ ;[Red]\-0\ </c:formatCode>
                 <c:ptCount val="18"/>
@@ -530,7 +794,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'DENSO - Honda PS-33'!$D$3:$D$17</c:f>
+              <c:f>'DENSO - Honda PS-30'!$D$3:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
                 <c:ptCount val="15"/>
@@ -586,7 +850,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'DENSO - Honda PS-33'!$E$2</c:f>
+              <c:f>'DENSO - Honda PS-30'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -606,7 +870,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'DENSO - Honda PS-33'!$C$3:$C$20</c:f>
+              <c:f>'DENSO - Honda PS-30'!$C$3:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>0_ ;[Red]\-0\ </c:formatCode>
                 <c:ptCount val="18"/>
@@ -660,52 +924,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'DENSO - Honda PS-33'!$E$3:$E$17</c:f>
+              <c:f>'DENSO - Honda PS-30'!$E$3:$E$17</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
                 <c:ptCount val="15"/>
-                <c:pt idx="1">
-                  <c:v>1.1299999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.37</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.66</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.88</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.17</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.75</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.15</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.85</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4.0999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4.3899999999999997</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4.66</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>4.95</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -719,11 +941,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="63888000"/>
-        <c:axId val="65282432"/>
+        <c:axId val="73257728"/>
+        <c:axId val="73259264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="63888000"/>
+        <c:axId val="73257728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="70"/>
@@ -735,14 +957,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65282432"/>
+        <c:crossAx val="73259264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
         <c:minorUnit val="10"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65282432"/>
+        <c:axId val="73259264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -753,7 +975,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63888000"/>
+        <c:crossAx val="73257728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -800,7 +1022,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'HITACHI - PS60-01'!$D$2</c:f>
+              <c:f>'DENSO - Honda PS-33'!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -809,54 +1031,70 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="5"/>
+          </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'HITACHI - PS60-01'!$C$4:$C$13</c:f>
+              <c:f>'DENSO - Honda PS-33'!$C$3:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>0_ ;[Red]\-0\ </c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
+                <c:ptCount val="18"/>
+                <c:pt idx="1">
                   <c:v>-70</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>-60</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>-50</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>-40</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>-30</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>-20</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>-10</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>70</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'HITACHI - PS60-01'!$D$4:$D$13</c:f>
+              <c:f>'DENSO - Honda PS-33'!$D$3:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>5.19</c:v>
-                </c:pt>
+                <c:ptCount val="15"/>
                 <c:pt idx="1">
                   <c:v>5.19</c:v>
                 </c:pt>
@@ -882,6 +1120,21 @@
                   <c:v>5.19</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>5.19</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.19</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.19</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.19</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.19</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>5.19</c:v>
                 </c:pt>
               </c:numCache>
@@ -894,7 +1147,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'HITACHI - PS60-01'!$E$2</c:f>
+              <c:f>'DENSO - Honda PS-33'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -905,7 +1158,7 @@
           </c:tx>
           <c:marker>
             <c:symbol val="star"/>
-            <c:size val="5"/>
+            <c:size val="6"/>
           </c:marker>
           <c:trendline>
             <c:trendlineType val="linear"/>
@@ -914,78 +1167,105 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'HITACHI - PS60-01'!$C$4:$C$13</c:f>
+              <c:f>'DENSO - Honda PS-33'!$C$3:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>0_ ;[Red]\-0\ </c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
+                <c:ptCount val="18"/>
+                <c:pt idx="1">
                   <c:v>-70</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>-60</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>-50</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>-40</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>-30</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>-20</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>-10</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>70</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'HITACHI - PS60-01'!$E$4:$E$13</c:f>
+              <c:f>'DENSO - Honda PS-33'!$E$3:$E$17</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1.48</c:v>
-                </c:pt>
+                <c:ptCount val="15"/>
                 <c:pt idx="1">
-                  <c:v>1.75</c:v>
+                  <c:v>1.1299999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.15</c:v>
+                  <c:v>1.37</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.5499999999999998</c:v>
+                  <c:v>1.66</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.12</c:v>
+                  <c:v>1.88</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.6</c:v>
+                  <c:v>2.17</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.55</c:v>
+                  <c:v>2.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.96</c:v>
+                  <c:v>3.15</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.18</c:v>
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.85</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.3899999999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.66</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.95</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1000,41 +1280,41 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="65308544"/>
-        <c:axId val="65310080"/>
+        <c:axId val="44494208"/>
+        <c:axId val="44573824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65308544"/>
+        <c:axId val="44494208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="30"/>
+          <c:max val="70"/>
           <c:min val="-80"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="0_ ;[Red]\-0\ " sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65310080"/>
+        <c:crossAx val="44573824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
         <c:minorUnit val="10"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65310080"/>
+        <c:axId val="44573824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00_ ;[Red]\-0.00\ " sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65308544"/>
+        <c:crossAx val="44494208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1050,7 +1330,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1081,7 +1361,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'DENSO 12R-3'!$D$3</c:f>
+              <c:f>'HITACHI - Subaru PS60-01'!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1090,16 +1370,12 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="diamond"/>
-            <c:size val="6"/>
-          </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'DENSO 12R-3'!$C$5:$C$26</c:f>
+              <c:f>'HITACHI - Subaru PS60-01'!$C$4:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>0_ ;[Red]\-0\ </c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>-70</c:v>
                 </c:pt>
@@ -1129,117 +1405,45 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>140</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'DENSO 12R-3'!$D$5:$D$26</c:f>
+              <c:f>'HITACHI - Subaru PS60-01'!$D$4:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>5.2</c:v>
+                  <c:v>5.19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.2</c:v>
+                  <c:v>5.19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.2</c:v>
+                  <c:v>5.19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.2</c:v>
+                  <c:v>5.19</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.2</c:v>
+                  <c:v>5.19</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.2</c:v>
+                  <c:v>5.19</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.2</c:v>
+                  <c:v>5.19</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.2</c:v>
+                  <c:v>5.19</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.2</c:v>
+                  <c:v>5.19</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5.2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5.2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5.2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5.2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>5.2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5.2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>5.2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>5.2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>5.2</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>5.2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>5.2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>5.2</c:v>
+                  <c:v>5.19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1251,7 +1455,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'DENSO 12R-3'!$E$3</c:f>
+              <c:f>'HITACHI - Subaru PS60-01'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1271,10 +1475,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'DENSO 12R-3'!$C$5:$C$26</c:f>
+              <c:f>'HITACHI - Subaru PS60-01'!$C$4:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>0_ ;[Red]\-0\ </c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>-70</c:v>
                 </c:pt>
@@ -1304,117 +1508,45 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>130</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>140</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'DENSO 12R-3'!$E$5:$E$26</c:f>
+              <c:f>'HITACHI - Subaru PS60-01'!$E$4:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.35</c:v>
+                  <c:v>1.48</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.44</c:v>
+                  <c:v>1.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6</c:v>
+                  <c:v>2.15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.75</c:v>
+                  <c:v>2.5499999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.93</c:v>
+                  <c:v>3.12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.1</c:v>
+                  <c:v>3.6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.2200000000000002</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.44</c:v>
+                  <c:v>4.55</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.64</c:v>
+                  <c:v>4.96</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.76</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2.93</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3.05</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3.21</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3.37</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.51</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3.65</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3.8</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3.98</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4.0999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>4.24</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>4.3899999999999997</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>4.51</c:v>
+                  <c:v>5.18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1429,14 +1561,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="70974080"/>
-        <c:axId val="70992256"/>
+        <c:axId val="44604032"/>
+        <c:axId val="44618112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="70974080"/>
+        <c:axId val="44604032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="150"/>
+          <c:max val="30"/>
           <c:min val="-80"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1445,14 +1577,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70992256"/>
+        <c:crossAx val="44618112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
         <c:minorUnit val="10"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="70992256"/>
+        <c:axId val="44618112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1463,7 +1595,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70974080"/>
+        <c:crossAx val="44604032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1510,7 +1642,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'OKI ELECTRIC'!$D$2</c:f>
+              <c:f>'DENSO - Subaru 12R13'!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1519,98 +1651,156 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+          </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'OKI ELECTRIC'!$C$4:$C$16</c:f>
+              <c:f>'DENSO - Subaru 12R13'!$C$5:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>0_ ;[Red]\-0\ </c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
+                  <c:v>-70</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>-60</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>-50</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>-40</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>-30</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>-20</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>-10</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>140</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'OKI ELECTRIC'!$D$4:$D$16</c:f>
+              <c:f>'DENSO - Subaru 12R13'!$D$5:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>5.18</c:v>
+                  <c:v>5.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.18</c:v>
+                  <c:v>5.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.18</c:v>
+                  <c:v>5.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.18</c:v>
+                  <c:v>5.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.18</c:v>
+                  <c:v>5.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.18</c:v>
+                  <c:v>5.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.18</c:v>
+                  <c:v>5.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.18</c:v>
+                  <c:v>5.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.18</c:v>
+                  <c:v>5.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.18</c:v>
+                  <c:v>5.2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.18</c:v>
+                  <c:v>5.2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.18</c:v>
+                  <c:v>5.2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.18</c:v>
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1622,7 +1812,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'OKI ELECTRIC'!$E$2</c:f>
+              <c:f>'DENSO - Subaru 12R13'!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1642,96 +1832,150 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'OKI ELECTRIC'!$C$4:$C$16</c:f>
+              <c:f>'DENSO - Subaru 12R13'!$C$5:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>0_ ;[Red]\-0\ </c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
+                  <c:v>-70</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>-60</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>-50</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>-40</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>-30</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>-20</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>-10</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>140</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'OKI ELECTRIC'!$E$4:$E$16</c:f>
+              <c:f>'DENSO - Subaru 12R13'!$E$5:$E$26</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>1.32</c:v>
+                  <c:v>1.35</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.57</c:v>
+                  <c:v>1.44</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.87</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.2000000000000002</c:v>
+                  <c:v>1.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.4500000000000002</c:v>
+                  <c:v>1.93</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.7</c:v>
+                  <c:v>2.1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.09</c:v>
+                  <c:v>2.2200000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.46</c:v>
+                  <c:v>2.44</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.79</c:v>
+                  <c:v>2.64</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4</c:v>
+                  <c:v>2.76</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.3</c:v>
+                  <c:v>2.93</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.46</c:v>
+                  <c:v>3.05</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.4000000000000004</c:v>
+                  <c:v>3.21</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.37</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.51</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.65</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.98</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.24</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.3899999999999997</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.51</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1746,15 +1990,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="71025024"/>
-        <c:axId val="71026560"/>
+        <c:axId val="55053696"/>
+        <c:axId val="55067776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71025024"/>
+        <c:axId val="55053696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="70"/>
-          <c:min val="-70"/>
+          <c:max val="150"/>
+          <c:min val="-80"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1762,14 +2006,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71026560"/>
+        <c:crossAx val="55067776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
         <c:minorUnit val="10"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71026560"/>
+        <c:axId val="55067776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1780,7 +2024,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71025024"/>
+        <c:crossAx val="55053696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1827,7 +2071,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'DENSO - 10M02'!$D$2</c:f>
+              <c:f>'OKI - Honda MNS-151'!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1838,10 +2082,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'DENSO - 10M02'!$C$4:$C$22</c:f>
+              <c:f>'OKI - Honda MNS-151'!$C$4:$C$16</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:formatCode>0_ ;[Red]\-0\ </c:formatCode>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>-60</c:v>
                 </c:pt>
@@ -1880,34 +2124,16 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>120</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'DENSO - 10M02'!$D$4:$D$22</c:f>
+              <c:f>'OKI - Honda MNS-151'!$D$4:$D$16</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>5.18</c:v>
                 </c:pt>
@@ -1945,24 +2171,6 @@
                   <c:v>5.18</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.18</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5.18</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>5.18</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5.18</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>5.18</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>5.18</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>5.18</c:v>
                 </c:pt>
               </c:numCache>
@@ -1975,7 +2183,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'DENSO - 10M02'!$E$2</c:f>
+              <c:f>'OKI - Honda MNS-151'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1995,10 +2203,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'DENSO - 10M02'!$C$4:$C$22</c:f>
+              <c:f>'OKI - Honda MNS-151'!$C$4:$C$16</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:formatCode>0_ ;[Red]\-0\ </c:formatCode>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>-60</c:v>
                 </c:pt>
@@ -2037,90 +2245,54 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>120</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'DENSO - 10M02'!$E$4:$E$22</c:f>
+              <c:f>'OKI - Honda MNS-151'!$E$4:$E$16</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>0.13</c:v>
+                  <c:v>1.32</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.28000000000000003</c:v>
+                  <c:v>1.57</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.53</c:v>
+                  <c:v>1.87</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.82</c:v>
+                  <c:v>2.2000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.1000000000000001</c:v>
+                  <c:v>2.4500000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4</c:v>
+                  <c:v>2.7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.65</c:v>
+                  <c:v>3.09</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.02</c:v>
+                  <c:v>3.46</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.35</c:v>
+                  <c:v>3.79</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.58</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.88</c:v>
+                  <c:v>4.3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.15</c:v>
+                  <c:v>4.46</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.42</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3.7</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.96</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>4.2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>4.55</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>4.76</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>5.09</c:v>
+                  <c:v>4.4000000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2135,11 +2307,400 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="72221440"/>
-        <c:axId val="72222976"/>
+        <c:axId val="55100544"/>
+        <c:axId val="55102080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72221440"/>
+        <c:axId val="55100544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="70"/>
+          <c:min val="-70"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0_ ;[Red]\-0\ " sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="55102080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="10"/>
+        <c:minorUnit val="10"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="55102080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00_ ;[Red]\-0.00\ " sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="55100544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-NZ"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'DENSO - Toyota 10M02'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Voltage In</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'DENSO - Toyota 10M02'!$C$4:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>-60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'DENSO - Toyota 10M02'!$D$4:$D$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>5.18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.18</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.18</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.18</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.18</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.18</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.18</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.18</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'DENSO - Toyota 10M02'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sensor Vout</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="star"/>
+            <c:size val="5"/>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'DENSO - Toyota 10M02'!$C$4:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>-60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'DENSO - Toyota 10M02'!$E$4:$E$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.65</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.02</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.35</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.58</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.88</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.15</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.42</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.96</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.55</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.76</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.09</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="55316864"/>
+        <c:axId val="55318400"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="55316864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="70"/>
@@ -2151,14 +2712,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72222976"/>
+        <c:crossAx val="55318400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
         <c:minorUnit val="10"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72222976"/>
+        <c:axId val="55318400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2169,7 +2730,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72221440"/>
+        <c:crossAx val="55316864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2301,8 +2862,10 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2320,6 +2883,85 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>499110</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>59055</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5490210" y="3800475"/>
+          <a:ext cx="3901440" cy="2926080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2351,10 +2993,54 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5600700" y="3810000"/>
+          <a:ext cx="3901440" cy="2926080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2386,10 +3072,54 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5524500" y="4191000"/>
+          <a:ext cx="3901440" cy="2926080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2421,10 +3151,54 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5581650" y="3931920"/>
+          <a:ext cx="3901440" cy="2926080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2747,11 +3521,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2790,7 +3564,7 @@
     </row>
     <row r="3" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
@@ -2857,13 +3631,13 @@
     </row>
     <row r="7" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
-      <c r="C7" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="25"/>
+      <c r="C7" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="26"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
@@ -2873,11 +3647,11 @@
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="28"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="29"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
@@ -2887,11 +3661,11 @@
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="28"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="29"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
@@ -2901,11 +3675,11 @@
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="28"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="29"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
@@ -2915,11 +3689,11 @@
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="28"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="29"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
@@ -2929,11 +3703,11 @@
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="28"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="29"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
@@ -2943,11 +3717,11 @@
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="28"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="29"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
@@ -2957,11 +3731,11 @@
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="28"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="29"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
@@ -2971,11 +3745,11 @@
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="28"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="29"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
@@ -2985,11 +3759,11 @@
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="28"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="29"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
@@ -2999,11 +3773,11 @@
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="28"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="29"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
@@ -3013,11 +3787,11 @@
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="28"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="29"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
@@ -3027,11 +3801,11 @@
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="28"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="29"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
@@ -3041,11 +3815,11 @@
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="28"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="29"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
@@ -3055,11 +3829,11 @@
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="28"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="29"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
@@ -3069,11 +3843,11 @@
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="28"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="29"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
@@ -3083,11 +3857,11 @@
     </row>
     <row r="23" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="6"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="31"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="32"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
@@ -3116,8 +3890,9 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <webPublishItems count="1">
-    <webPublishItem id="29651" divId="MAP Sensor Data_29651" sourceType="sheet" destinationFile="C:\Users\el_presto\Desktop\WorkSpace\FreeEMS\MAP_SensorData.htm" autoRepublish="1"/>
+    <webPublishItem id="311" divId="MAP Sensor Data_311" sourceType="sheet" destinationFile="C:\Users\el_presto\Desktop\WorkSpace\FreeEMS\MapSensors\MapSensorData.mht" title="MAP Sensor Data" autoRepublish="1"/>
   </webPublishItems>
 </worksheet>
 </file>
@@ -3127,7 +3902,313 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D4" sqref="D4:D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="14" width="9.140625" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <f>('ATM Data'!$E$5+C4)</f>
+        <v>32.27000000000001</v>
+      </c>
+      <c r="C4" s="15">
+        <v>-70</v>
+      </c>
+      <c r="D4" s="13">
+        <v>5.19</v>
+      </c>
+      <c r="E4" s="13"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <f>('ATM Data'!$E$5+C5)</f>
+        <v>42.27000000000001</v>
+      </c>
+      <c r="C5" s="15">
+        <v>-60</v>
+      </c>
+      <c r="D5" s="13">
+        <v>5.19</v>
+      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <f>('ATM Data'!$E$5+C6)</f>
+        <v>52.27000000000001</v>
+      </c>
+      <c r="C6" s="15">
+        <v>-50</v>
+      </c>
+      <c r="D6" s="13">
+        <v>5.19</v>
+      </c>
+      <c r="E6" s="13"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f>('ATM Data'!$E$5+C7)</f>
+        <v>62.27000000000001</v>
+      </c>
+      <c r="C7" s="15">
+        <v>-40</v>
+      </c>
+      <c r="D7" s="13">
+        <v>5.19</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f>('ATM Data'!$E$5+C8)</f>
+        <v>72.27000000000001</v>
+      </c>
+      <c r="C8" s="15">
+        <v>-30</v>
+      </c>
+      <c r="D8" s="13">
+        <v>5.19</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <f>('ATM Data'!$E$5+C9)</f>
+        <v>82.27000000000001</v>
+      </c>
+      <c r="C9" s="15">
+        <v>-20</v>
+      </c>
+      <c r="D9" s="13">
+        <v>5.19</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <f>('ATM Data'!$E$5+C10)</f>
+        <v>92.27000000000001</v>
+      </c>
+      <c r="C10" s="15">
+        <v>-10</v>
+      </c>
+      <c r="D10" s="13">
+        <v>5.19</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="5">
+        <f>('ATM Data'!$E$5+C11)</f>
+        <v>102.27000000000001</v>
+      </c>
+      <c r="C11" s="16">
+        <v>0</v>
+      </c>
+      <c r="D11" s="14">
+        <v>5.19</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <f>('ATM Data'!$E$5+C12)</f>
+        <v>112.27000000000001</v>
+      </c>
+      <c r="C12" s="15">
+        <v>10</v>
+      </c>
+      <c r="D12" s="13">
+        <v>5.19</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <f>('ATM Data'!$E$5+C13)</f>
+        <v>122.27000000000001</v>
+      </c>
+      <c r="C13" s="15">
+        <v>20</v>
+      </c>
+      <c r="D13" s="13">
+        <v>5.19</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <f>('ATM Data'!$E$5+C14)</f>
+        <v>132.27000000000001</v>
+      </c>
+      <c r="C14" s="15">
+        <v>30</v>
+      </c>
+      <c r="D14" s="13">
+        <v>5.19</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <f>('ATM Data'!$E$5+C15)</f>
+        <v>142.27000000000001</v>
+      </c>
+      <c r="C15" s="15">
+        <v>40</v>
+      </c>
+      <c r="D15" s="13">
+        <v>5.19</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f>('ATM Data'!$E$5+C16)</f>
+        <v>152.27000000000001</v>
+      </c>
+      <c r="C16" s="15">
+        <v>50</v>
+      </c>
+      <c r="D16" s="13">
+        <v>5.19</v>
+      </c>
+      <c r="E16" s="13"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <f>('ATM Data'!$E$5+C17)</f>
+        <v>162.27000000000001</v>
+      </c>
+      <c r="C17" s="15">
+        <v>60</v>
+      </c>
+      <c r="D17" s="13">
+        <v>5.19</v>
+      </c>
+      <c r="E17" s="13"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <f>('ATM Data'!$E$5+C18)</f>
+        <v>172.27</v>
+      </c>
+      <c r="C18" s="15">
+        <v>70</v>
+      </c>
+      <c r="D18" s="13">
+        <v>5.19</v>
+      </c>
+      <c r="E18" s="13"/>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="33"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="33"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="G22" s="36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="33"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A20:E23"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="G22" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="8" orientation="landscape" r:id="rId3"/>
+  <drawing r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N39"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -3162,7 +4243,9 @@
       <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="35" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3376,7 +4459,7 @@
       </c>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>('ATM Data'!$E$5+C17)</f>
         <v>162.27000000000001</v>
@@ -3392,7 +4475,7 @@
       </c>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18">
         <f>('ATM Data'!$E$5+C18)</f>
         <v>172.27</v>
@@ -3408,53 +4491,185 @@
       </c>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="32"/>
-      <c r="B21" s="32"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="32"/>
-      <c r="B23" s="32"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="33"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="33"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="G22" s="36"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="33"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="G23" s="36"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="33"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="G24" s="36"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="33"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="G25" s="36"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="33"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="G26" s="36"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="33"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="G27" s="36"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="33"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="G28" s="36"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="33"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="G29" s="36"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="33"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="G30" s="36"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="33"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="G31" s="36"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="33"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="G32" s="36"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="33"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+      <c r="G33" s="36"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="33"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
+      <c r="G34" s="36"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="33"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
+      <c r="G35" s="36"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="33"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
+      <c r="G36" s="36"/>
+    </row>
+    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="33"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="33"/>
+      <c r="G37" s="36"/>
+    </row>
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="33"/>
+      <c r="B38" s="33"/>
+      <c r="C38" s="33"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="33"/>
+      <c r="G38" s="36"/>
+    </row>
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="33"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A20:E23"/>
+    <mergeCell ref="A20:E39"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="8" orientation="landscape" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -3648,40 +4863,147 @@
     <row r="15" spans="1:5" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
+      <c r="A17" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="32"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25"/>
+      <c r="A20" s="33"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="33"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="33"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="33"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="33"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="33"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="33"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="33"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="33"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="33"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="33"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="33"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="33"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="33"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="33"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="33"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G36" s="36"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A17:E20"/>
+    <mergeCell ref="A17:E35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
@@ -3689,12 +5011,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23:L26"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -3915,7 +5237,7 @@
         <v>3.05</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B17" s="7">
         <f>('ATM Data'!$E$5+C17)</f>
         <v>152.27000000000001</v>
@@ -3930,7 +5252,7 @@
         <v>3.21</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B18" s="7">
         <f>('ATM Data'!$E$5+C18)</f>
         <v>162.27000000000001</v>
@@ -3945,7 +5267,7 @@
         <v>3.37</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B19" s="7">
         <f>('ATM Data'!$E$5+C19)</f>
         <v>172.27</v>
@@ -3960,7 +5282,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B20" s="7">
         <f>('ATM Data'!$E$5+C20)</f>
         <v>182.27</v>
@@ -3975,7 +5297,7 @@
         <v>3.65</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B21" s="7">
         <f>('ATM Data'!$E$5+C21)</f>
         <v>192.27</v>
@@ -3990,7 +5312,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B22" s="7">
         <f>('ATM Data'!$E$5+C22)</f>
         <v>202.27</v>
@@ -4005,7 +5327,7 @@
         <v>3.98</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B23" s="7">
         <f>('ATM Data'!$E$5+C23)</f>
         <v>212.27</v>
@@ -4019,16 +5341,8 @@
       <c r="E23" s="17">
         <v>4.0999999999999996</v>
       </c>
-      <c r="G23" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="33"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B24" s="7">
         <f>('ATM Data'!$E$5+C24)</f>
         <v>222.27</v>
@@ -4042,14 +5356,8 @@
       <c r="E24" s="17">
         <v>4.24</v>
       </c>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B25" s="7">
         <f>('ATM Data'!$E$5+C25)</f>
         <v>232.27</v>
@@ -4063,14 +5371,8 @@
       <c r="E25" s="17">
         <v>4.3899999999999997</v>
       </c>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="33"/>
-      <c r="K25" s="33"/>
-      <c r="L25" s="33"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B26" s="7">
         <f>('ATM Data'!$E$5+C26)</f>
         <v>242.27</v>
@@ -4084,18 +5386,206 @@
       <c r="E26" s="17">
         <v>4.51</v>
       </c>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="33"/>
-      <c r="K26" s="33"/>
-      <c r="L26" s="33"/>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="7"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="34"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="34"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="34"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="23"/>
+      <c r="L30" s="23"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="34"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="23"/>
+      <c r="K31" s="23"/>
+      <c r="L31" s="23"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="34"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="34"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="23"/>
+      <c r="L33" s="23"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="34"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="23"/>
+      <c r="K34" s="23"/>
+      <c r="L34" s="23"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="34"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="23"/>
+      <c r="K35" s="23"/>
+      <c r="L35" s="23"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="34"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="23"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="23"/>
+      <c r="K36" s="23"/>
+      <c r="L36" s="23"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="34"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="34"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="23"/>
+      <c r="J37" s="23"/>
+      <c r="K37" s="23"/>
+      <c r="L37" s="23"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="34"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="23"/>
+      <c r="J38" s="23"/>
+      <c r="K38" s="23"/>
+      <c r="L38" s="23"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="34"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="23"/>
+      <c r="J39" s="23"/>
+      <c r="K39" s="23"/>
+      <c r="L39" s="23"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="34"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="23"/>
+      <c r="J40" s="23"/>
+      <c r="K40" s="23"/>
+      <c r="L40" s="23"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="34"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="34"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="34"/>
+      <c r="G41" s="36"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G23:L26"/>
+    <mergeCell ref="A28:E41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
@@ -4103,12 +5593,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:E21"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -4343,37 +5833,168 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="34"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="34"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="34"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="34"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="34"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="34"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="34"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="34"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="34"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="34"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="34"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="34"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="34"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="34"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="34"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="34"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="34"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="34"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="34"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="34"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="34"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="G39" s="36"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B18:E21"/>
+    <mergeCell ref="A18:E39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
@@ -4381,12 +6002,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -4621,7 +6242,7 @@
         <v>3.42</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" s="7">
         <f>('ATM Data'!$E$5+C17)</f>
         <v>172.27</v>
@@ -4636,7 +6257,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" s="7">
         <f>('ATM Data'!$E$5+C18)</f>
         <v>182.27</v>
@@ -4651,7 +6272,7 @@
         <v>3.96</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="7">
         <f>('ATM Data'!$E$5+C19)</f>
         <v>192.27</v>
@@ -4666,7 +6287,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="7">
         <f>('ATM Data'!$E$5+C20)</f>
         <v>202.27</v>
@@ -4681,7 +6302,7 @@
         <v>4.55</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="7">
         <f>('ATM Data'!$E$5+C21)</f>
         <v>212.27</v>
@@ -4695,16 +6316,8 @@
       <c r="E21">
         <v>4.76</v>
       </c>
-      <c r="G21" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="7">
         <f>('ATM Data'!$E$5+C22)</f>
         <v>222.27</v>
@@ -4718,32 +6331,151 @@
       <c r="E22">
         <v>5.09</v>
       </c>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="33"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="7"/>
+    </row>
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="37"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="33"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="37"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="33"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="37"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="33"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="37"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="33"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="37"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="33"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="37"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="33"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="37"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="33"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="37"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="33"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="37"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="33"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="37"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="33"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="37"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="33"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="37"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="33"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="37"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="37"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+    </row>
+    <row r="38" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="37"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="37"/>
+    </row>
+    <row r="39" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="37"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="37"/>
+    </row>
+    <row r="40" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="37"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="37"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G21:L24"/>
+    <mergeCell ref="A24:E36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Added img to and data to PS-30, updated todo, updated pdf.
</commit_message>
<xml_diff>
--- a/MAP Sensor Data.xlsx
+++ b/MAP Sensor Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="12255" windowHeight="7005"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="12255" windowHeight="7005" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ATM Data" sheetId="6" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="17">
   <si>
     <t>hPa</t>
   </si>
@@ -124,14 +124,6 @@
   </si>
   <si>
     <t>Sensor_img\DENSO_Honda_PS-33.JPG</t>
-  </si>
-  <si>
-    <t>Sensor_img\DENSO_Honda_PS-30.JPG</t>
-  </si>
-  <si>
-    <t>**Testing Notes**
- - Donner vehicle = Honda NA engine (Manifold/throttle body mounted)
- - Part #</t>
   </si>
   <si>
     <t>**Testing Notes**
@@ -375,6 +367,21 @@
                    - YR ---&gt; GW = 4.00kΩ
 - MAP Test date : 24-12-2011 @ 2300hrs : 1022 hPa</t>
     </r>
+  </si>
+  <si>
+    <t>**Testing Notes**
+ - Donner vehicle = Honda NA engine (Manifold/throttle body mounted)
+  - Part # 079800-3280
+ - Voltage rating: 5V
+ - Wire colour coding :
+                   - Red with Green Strip (RG) = V+
+                   - Yellow with Red Strip (YR) = Vout
+                   - Greenn with White Strip (GW) = GND
+- Measured Resistance Readings :
+                   - RG ---&gt; YR = X.XXkΩ
+                   - RG ---&gt; GW = X.XXkΩ
+                   - YR ---&gt; GW = X.XXkΩ
+- MAP Test date : 24-12-2011 @ 2115hrs : 1022 hPa</t>
   </si>
 </sst>
 </file>
@@ -2877,6 +2884,50 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5600700" y="4000500"/>
+          <a:ext cx="3901440" cy="2926080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3524,7 +3575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -3899,10 +3950,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D18"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -4127,7 +4178,7 @@
       <c r="E16" s="13"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>('ATM Data'!$E$5+C17)</f>
         <v>162.27000000000001</v>
@@ -4141,7 +4192,7 @@
       <c r="E17" s="13"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18">
         <f>('ATM Data'!$E$5+C18)</f>
         <v>172.27</v>
@@ -4155,51 +4206,174 @@
       <c r="E18" s="13"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="33" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B20" s="33"/>
       <c r="C20" s="33"/>
       <c r="D20" s="33"/>
       <c r="E20" s="33"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="33"/>
       <c r="B21" s="33"/>
       <c r="C21" s="33"/>
       <c r="D21" s="33"/>
       <c r="E21" s="33"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="33"/>
       <c r="B22" s="33"/>
       <c r="C22" s="33"/>
       <c r="D22" s="33"/>
       <c r="E22" s="33"/>
-      <c r="G22" s="36" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="33"/>
       <c r="B23" s="33"/>
       <c r="C23" s="33"/>
       <c r="D23" s="33"/>
       <c r="E23" s="33"/>
     </row>
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="33"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+    </row>
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="33"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+    </row>
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="33"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+    </row>
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="33"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+    </row>
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="33"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+    </row>
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="33"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+    </row>
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="33"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+    </row>
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="33"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+    </row>
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="33"/>
+      <c r="B32" s="33"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+    </row>
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="33"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+    </row>
+    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="33"/>
+      <c r="B34" s="33"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="33"/>
+    </row>
+    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="33"/>
+      <c r="B35" s="33"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
+    </row>
+    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="33"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
+    </row>
+    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="33"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="33"/>
+    </row>
+    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="33"/>
+      <c r="B38" s="33"/>
+      <c r="C38" s="33"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="33"/>
+    </row>
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="33"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="33"/>
+    </row>
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="33"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
+      <c r="G40" s="36"/>
+    </row>
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="33"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="33"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="33"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A20:E23"/>
+    <mergeCell ref="A20:E41"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="G22" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" orientation="landscape" r:id="rId3"/>
-  <drawing r:id="rId4"/>
+  <pageSetup paperSize="8" orientation="landscape" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -4494,7 +4668,7 @@
     <row r="19" spans="1:7" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="33" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B20" s="33"/>
       <c r="C20" s="33"/>
@@ -4864,7 +5038,7 @@
     <row r="16" spans="1:5" x14ac:dyDescent="0.25"/>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="33"/>
@@ -5401,7 +5575,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B28" s="34"/>
       <c r="C28" s="34"/>
@@ -5836,7 +6010,7 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B18" s="34"/>
       <c r="C18" s="34"/>

</xml_diff>